<commit_message>
use new agile system lca features
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-2.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/oilcane_spearman_-2.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE37"/>
+  <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -734,44 +734,44 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.02694410421376417</v>
+        <v>0.001518318108732724</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.006983176887327074</v>
+        <v>0.002440304641612186</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>0.007878156027126239</v>
+        <v>0.0008292941131717646</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0140078803874164</v>
+        <v>0.003172265145129379</v>
       </c>
       <c r="H4" t="n">
-        <v>0.001345616981824679</v>
+        <v>-0.01685983094639324</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.007449268809970751</v>
+        <v>0.004083328675333147</v>
       </c>
       <c r="J4" t="n">
-        <v>0.006503007806244199</v>
+        <v>0.01208809448016959</v>
       </c>
       <c r="K4" t="n">
-        <v>0.002172098198883927</v>
+        <v>-0.01760355536014221</v>
       </c>
       <c r="L4" t="n">
-        <v>0.002172098198883927</v>
+        <v>-0.01760355536014221</v>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
-        <v>0.002172678710907148</v>
+        <v>-0.01760414470416579</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.002172293078891723</v>
+        <v>-0.01760355536014221</v>
       </c>
       <c r="R4" t="n">
-        <v>0.002172293078891723</v>
+        <v>-0.01760355536014221</v>
       </c>
       <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
@@ -795,44 +795,44 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.01275197571007903</v>
+        <v>-0.009220427408817095</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0005059528522381141</v>
+        <v>-0.01886649176265967</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>-0.00715142476605699</v>
+        <v>0.01930894176435767</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.01701600986265392</v>
+        <v>0.01062561738827025</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.005894852299794092</v>
+        <v>0.004125332517013301</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.001284875859395034</v>
+        <v>-0.009963135470525417</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.004009940741568771</v>
+        <v>0.01626895867631969</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.002111571924462876</v>
+        <v>-0.005391140471645618</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.002111571924462876</v>
+        <v>-0.005391140471645618</v>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
-        <v>-0.002110957332438293</v>
+        <v>-0.005390941655637665</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.002111315028452601</v>
+        <v>-0.005391140471645618</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.002111315028452601</v>
+        <v>-0.005391140471645618</v>
       </c>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
@@ -856,44 +856,44 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1938094353363774</v>
+        <v>0.2103740895989636</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9579628848145153</v>
+        <v>0.9579101443324056</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>0.004457707858308313</v>
+        <v>-0.003546465357858613</v>
       </c>
       <c r="G6" t="n">
-        <v>0.002663232490579546</v>
+        <v>0.03505249070660543</v>
       </c>
       <c r="H6" t="n">
-        <v>0.000161164326446573</v>
+        <v>0.0002018905040756201</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9580282262571288</v>
+        <v>0.9570899158835965</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.01135456255135341</v>
+        <v>-0.006947756352317192</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.004223912232956489</v>
+        <v>-0.001628774177150967</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.004223912232956489</v>
+        <v>-0.001628774177150967</v>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
-        <v>-0.004223184072927363</v>
+        <v>-0.001628421857136874</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.004223637096945483</v>
+        <v>-0.001628774177150967</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.004223637096945483</v>
+        <v>-0.001628774177150967</v>
       </c>
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
@@ -921,44 +921,44 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.9288805593632223</v>
+        <v>0.9294598989383958</v>
       </c>
       <c r="D7" t="n">
-        <v>0.001493300027732001</v>
+        <v>0.02428762417150496</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>-0.003826080825043232</v>
+        <v>0.01695514330220573</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0002434976846411658</v>
+        <v>0.009917860814668489</v>
       </c>
       <c r="H7" t="n">
-        <v>0.01457700288708011</v>
+        <v>0.01928205379528215</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.00204288776171551</v>
+        <v>0.0245176349967054</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.009129700495102859</v>
+        <v>0.01577294147745551</v>
       </c>
       <c r="K7" t="n">
-        <v>0.02115705281428211</v>
+        <v>0.01564757640190306</v>
       </c>
       <c r="L7" t="n">
-        <v>0.02115705281428211</v>
+        <v>0.01564757640190306</v>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
-        <v>0.0211581549903262</v>
+        <v>0.01564801377792055</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.02115713988628559</v>
+        <v>0.01564757640190306</v>
       </c>
       <c r="R7" t="n">
-        <v>0.02115713988628559</v>
+        <v>0.01564757640190306</v>
       </c>
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
@@ -986,44 +986,44 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.01257454187898167</v>
+        <v>-0.02895015043800602</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.009443602841744113</v>
+        <v>-0.01683367161734686</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>-0.01134134790965392</v>
+        <v>0.005270560722822428</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01354971976888972</v>
+        <v>0.006968239646127269</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.0222708800908352</v>
+        <v>-0.003981588543263541</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.01020379029615161</v>
+        <v>-0.01207669382706775</v>
       </c>
       <c r="J8" t="n">
-        <v>0.008582789613610036</v>
+        <v>0.002494442699214203</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.02208150635526025</v>
+        <v>-0.005448456985938279</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.02208150635526025</v>
+        <v>-0.005448456985938279</v>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="n">
-        <v>-0.02208222203528888</v>
+        <v>-0.005448544441941777</v>
       </c>
       <c r="Q8" t="n">
-        <v>-0.0220815275712611</v>
+        <v>-0.005448456985938279</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.0220815275712611</v>
+        <v>-0.005448456985938279</v>
       </c>
       <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
@@ -1051,44 +1051,44 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.01802489668899587</v>
+        <v>-0.006618980424759216</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02935640968625638</v>
+        <v>0.01662563970502559</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>-0.02956419180656767</v>
+        <v>-0.02551162710046508</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.01351894534502476</v>
+        <v>0.003883925985944186</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.0180361050734442</v>
+        <v>-0.0196022574880903</v>
       </c>
       <c r="I9" t="n">
-        <v>0.02196674103866964</v>
+        <v>0.01769320726772829</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.01491610718546241</v>
+        <v>0.0004712809253249844</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.01361091952043678</v>
+        <v>-0.01513272281330891</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.01361091952043678</v>
+        <v>-0.01513272281330891</v>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
-        <v>-0.01361067971242719</v>
+        <v>-0.01513336418933457</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.01361118812844752</v>
+        <v>-0.01513272281330891</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.01361118812844752</v>
+        <v>-0.01513272281330891</v>
       </c>
       <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
@@ -1116,44 +1116,44 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.0110135975605439</v>
+        <v>-0.001780981319239252</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0009429528377181134</v>
+        <v>-0.00196987025479481</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>0.009974146862965874</v>
+        <v>0.008045883777835352</v>
       </c>
       <c r="G10" t="n">
-        <v>0.007723849665543396</v>
+        <v>-0.004660722670756902</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.005463013946520557</v>
+        <v>0.009574865086994603</v>
       </c>
       <c r="I10" t="n">
-        <v>0.002161791062471642</v>
+        <v>-0.003044800153792006</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.003161540113612717</v>
+        <v>0.01039168360661212</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.01010985582839423</v>
+        <v>0.007374535494981419</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.01010985582839423</v>
+        <v>0.007374535494981419</v>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
-        <v>-0.0101097874763915</v>
+        <v>0.007374741990989679</v>
       </c>
       <c r="Q10" t="n">
-        <v>-0.0101097900683916</v>
+        <v>0.007374535494981419</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.0101097900683916</v>
+        <v>0.007374535494981419</v>
       </c>
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
@@ -1177,44 +1177,44 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.122364901342596</v>
+        <v>0.1372878559875142</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2739322870212915</v>
+        <v>0.2654456043458241</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>-0.006009922032396881</v>
+        <v>-0.0007955465598218623</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.00973970541237041</v>
+        <v>-0.02127046048419651</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.006678716907148675</v>
+        <v>0.006166517142660685</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.001699226851969074</v>
+        <v>-0.01768428272337131</v>
       </c>
       <c r="J11" t="n">
-        <v>0.009512598438551529</v>
+        <v>-0.001140441478962831</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.00808353478734139</v>
+        <v>0.004345403885816155</v>
       </c>
       <c r="L11" t="n">
-        <v>-0.00808353478734139</v>
+        <v>0.004345403885816155</v>
       </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
-        <v>-0.008082972707318907</v>
+        <v>0.004345284365811373</v>
       </c>
       <c r="Q11" t="n">
-        <v>-0.008083260707330429</v>
+        <v>0.004345403885816155</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.008083260707330429</v>
+        <v>0.004345403885816155</v>
       </c>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
@@ -1238,44 +1238,44 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.2481897655115906</v>
+        <v>-0.23661700143268</v>
       </c>
       <c r="D12" t="n">
-        <v>0.00596510827060433</v>
+        <v>0.0006189252727570108</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>-0.005824556296982252</v>
+        <v>0.01250909358836374</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.008073181853630243</v>
+        <v>0.02147203260047696</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.0131086325243453</v>
+        <v>-0.001510393404415736</v>
       </c>
       <c r="I12" t="n">
-        <v>0.008871952386878094</v>
+        <v>-0.001257704210308168</v>
       </c>
       <c r="J12" t="n">
-        <v>0.006663781176089961</v>
+        <v>0.01328352908255431</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.01836409206256368</v>
+        <v>-0.004103684900147395</v>
       </c>
       <c r="L12" t="n">
-        <v>-0.01836409206256368</v>
+        <v>-0.004103684900147395</v>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
-        <v>-0.01836351951854077</v>
+        <v>-0.004103815460152619</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0183637224625489</v>
+        <v>-0.004103684900147395</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0183637224625489</v>
+        <v>-0.004103684900147395</v>
       </c>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -1303,44 +1303,44 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.01206733190669327</v>
+        <v>-0.007104360092174403</v>
       </c>
       <c r="D13" t="n">
-        <v>0.008566614198664566</v>
+        <v>-0.01166114235444569</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>-0.003576334799053391</v>
+        <v>0.00919050027162001</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.002308725814041237</v>
+        <v>-0.00986017332234088</v>
       </c>
       <c r="H13" t="n">
-        <v>0.007202975040119</v>
+        <v>-0.006150482550019301</v>
       </c>
       <c r="I13" t="n">
-        <v>0.01022208232888329</v>
+        <v>-0.01352679135707165</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.0006451569995094147</v>
+        <v>0.01820129719655752</v>
       </c>
       <c r="K13" t="n">
-        <v>0.01317420695896828</v>
+        <v>-0.01293926480557059</v>
       </c>
       <c r="L13" t="n">
-        <v>0.01317420695896828</v>
+        <v>-0.01293926480557059</v>
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
-        <v>0.01317437534297501</v>
+        <v>-0.01293987718959509</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.01317438187097527</v>
+        <v>-0.01293926480557059</v>
       </c>
       <c r="R13" t="n">
-        <v>0.01317438187097527</v>
+        <v>-0.01293926480557059</v>
       </c>
       <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
@@ -1368,44 +1368,44 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.004794905471796219</v>
+        <v>0.0103537975021519</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.007119685916787436</v>
+        <v>-0.0008059194562367781</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>-0.009668640578745622</v>
+        <v>0.04249710131588405</v>
       </c>
       <c r="G14" t="n">
-        <v>0.016418328172278</v>
+        <v>-0.01151252792932238</v>
       </c>
       <c r="H14" t="n">
-        <v>0.001014010696560427</v>
+        <v>0.03983173349726933</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.000965669702626788</v>
+        <v>-5.832729833309193e-05</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.01897468388200965</v>
+        <v>0.02761579952636551</v>
       </c>
       <c r="K14" t="n">
-        <v>0.00609401227576049</v>
+        <v>0.03334768914190756</v>
       </c>
       <c r="L14" t="n">
-        <v>0.00609401227576049</v>
+        <v>0.03334768914190756</v>
       </c>
       <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="n">
-        <v>0.006092855955714237</v>
+        <v>0.03334756894990275</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.006093900915756035</v>
+        <v>0.03334768914190756</v>
       </c>
       <c r="R14" t="n">
-        <v>0.006093900915756035</v>
+        <v>0.03334768914190756</v>
       </c>
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
@@ -1433,44 +1433,44 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.006910162740406509</v>
+        <v>-0.01367637174705487</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.01063130442525218</v>
+        <v>-0.009508359644334384</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>0.01469088538763541</v>
+        <v>0.006195038935801557</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.003237543957545683</v>
+        <v>0.005627387921306281</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00982271079290843</v>
+        <v>0.01774646691785867</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.006534425637377024</v>
+        <v>-0.006965626934625076</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.008043675420594684</v>
+        <v>-0.01198376013767749</v>
       </c>
       <c r="K15" t="n">
-        <v>0.008495334387813375</v>
+        <v>0.01646316382652655</v>
       </c>
       <c r="L15" t="n">
-        <v>0.008495334387813375</v>
+        <v>0.01646316382652655</v>
       </c>
       <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
-        <v>0.00849503073980123</v>
+        <v>0.01646302357052094</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.008495296755811869</v>
+        <v>0.01646316382652655</v>
       </c>
       <c r="R15" t="n">
-        <v>0.008495296755811869</v>
+        <v>0.01646316382652655</v>
       </c>
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
@@ -1498,44 +1498,44 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.02671727828469113</v>
+        <v>-0.03850821062832842</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01187364479494579</v>
+        <v>0.001442512665700506</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>-0.0004396648495865939</v>
+        <v>0.01063482628139305</v>
       </c>
       <c r="G16" t="n">
-        <v>0.006463134096842622</v>
+        <v>-0.03610644054995379</v>
       </c>
       <c r="H16" t="n">
-        <v>0.007200610560024421</v>
+        <v>0.0016738649949546</v>
       </c>
       <c r="I16" t="n">
-        <v>0.005726904229076169</v>
+        <v>-0.00457620200704808</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.006777764767070316</v>
+        <v>0.0118839691874681</v>
       </c>
       <c r="K16" t="n">
-        <v>0.005081456651258265</v>
+        <v>0.002074597234983889</v>
       </c>
       <c r="L16" t="n">
-        <v>0.005081456651258265</v>
+        <v>0.002074597234983889</v>
       </c>
       <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
-        <v>0.005081426891257075</v>
+        <v>0.002073996274959851</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.005081319947252797</v>
+        <v>0.002074597234983889</v>
       </c>
       <c r="R16" t="n">
-        <v>0.005081319947252797</v>
+        <v>0.002074597234983889</v>
       </c>
       <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr"/>
@@ -1559,44 +1559,44 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.002309634524385381</v>
+        <v>0.01272683830107353</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.006570467302818691</v>
+        <v>0.02845959675438387</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>-0.006801880592075223</v>
+        <v>-0.005951688334067532</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.00321283623122594</v>
+        <v>0.01875625817999487</v>
       </c>
       <c r="H17" t="n">
-        <v>-0.01323320980932839</v>
+        <v>0.003092654043706161</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0007193015327720613</v>
+        <v>0.02882727782509111</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.01626272821192948</v>
+        <v>-0.001526256430969781</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.01494317032572681</v>
+        <v>0.00402294726491789</v>
       </c>
       <c r="L17" t="n">
-        <v>-0.01494317032572681</v>
+        <v>0.00402294726491789</v>
       </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
-        <v>-0.01494330030973201</v>
+        <v>0.004022955616918224</v>
       </c>
       <c r="Q17" t="n">
-        <v>-0.01494336722173469</v>
+        <v>0.00402294726491789</v>
       </c>
       <c r="R17" t="n">
-        <v>-0.01494336722173469</v>
+        <v>0.00402294726491789</v>
       </c>
       <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr"/>
@@ -1624,44 +1624,44 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.06971249770049991</v>
+        <v>-0.03195523107020923</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.004741255389650215</v>
+        <v>0.004848441889937675</v>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>0.001983348463333938</v>
+        <v>0.01594002303760092</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0005964633648733071</v>
+        <v>-0.0002331509843615382</v>
       </c>
       <c r="H18" t="n">
-        <v>0.008496476019859039</v>
+        <v>0.002700124140004965</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1668378565935142</v>
+        <v>0.1819068643002746</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.01522442771634396</v>
+        <v>-0.001950206281349636</v>
       </c>
       <c r="K18" t="n">
-        <v>0.007817697336707893</v>
+        <v>-0.001576403967056158</v>
       </c>
       <c r="L18" t="n">
-        <v>0.007817697336707893</v>
+        <v>-0.001576403967056158</v>
       </c>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
-        <v>0.007818160152726406</v>
+        <v>-0.001576574079062963</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.007817563992702559</v>
+        <v>-0.001576403967056158</v>
       </c>
       <c r="R18" t="n">
-        <v>0.007817563992702559</v>
+        <v>-0.001576403967056158</v>
       </c>
       <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr"/>
@@ -1689,44 +1689,44 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.009769040262761609</v>
+        <v>0.01942644874505795</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.005024797256991891</v>
+        <v>0.003681679443267178</v>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>0.3477923373036935</v>
+        <v>0.3234155862486234</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.01514693122710279</v>
+        <v>0.02340809268300184</v>
       </c>
       <c r="H19" t="n">
-        <v>0.2449979400079176</v>
+        <v>0.2128371705294868</v>
       </c>
       <c r="I19" t="n">
-        <v>0.008145658213826328</v>
+        <v>0.01345383817015353</v>
       </c>
       <c r="J19" t="n">
-        <v>0.1843291762163188</v>
+        <v>0.1513832904116739</v>
       </c>
       <c r="K19" t="n">
-        <v>0.1779493536139741</v>
+        <v>0.1534878409875136</v>
       </c>
       <c r="L19" t="n">
-        <v>0.1779493536139741</v>
+        <v>0.1534878409875136</v>
       </c>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="n">
-        <v>0.1779486054859442</v>
+        <v>0.1534871962514879</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.1779493814539752</v>
+        <v>0.1534878409875136</v>
       </c>
       <c r="R19" t="n">
-        <v>0.1779493814539752</v>
+        <v>0.1534878409875136</v>
       </c>
       <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr"/>
@@ -1750,44 +1750,44 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.01084056148962246</v>
+        <v>-0.01281598304063932</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.006169556118782244</v>
+        <v>0.0001811943432477737</v>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>0.009340302997612118</v>
+        <v>0.01527973385918935</v>
       </c>
       <c r="G20" t="n">
-        <v>0.01455200875719432</v>
+        <v>-0.01366611155799702</v>
       </c>
       <c r="H20" t="n">
-        <v>0.005836704233468169</v>
+        <v>-0.008545546613821864</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.01076469134258765</v>
+        <v>-0.0001040154281606171</v>
       </c>
       <c r="J20" t="n">
-        <v>0.009141006175795221</v>
+        <v>0.00710496221809917</v>
       </c>
       <c r="K20" t="n">
-        <v>0.002491949859677994</v>
+        <v>-0.01402207976088319</v>
       </c>
       <c r="L20" t="n">
-        <v>0.002491949859677994</v>
+        <v>-0.01402207976088319</v>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="n">
-        <v>0.002491542915661716</v>
+        <v>-0.01402167656086706</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.002491994595679783</v>
+        <v>-0.01402207976088319</v>
       </c>
       <c r="R20" t="n">
-        <v>0.002491994595679783</v>
+        <v>-0.01402207976088319</v>
       </c>
       <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr"/>
@@ -1811,44 +1811,44 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.02624651480986059</v>
+        <v>0.05024914664996586</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.01017601365504055</v>
+        <v>-0.003839358873574354</v>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>0.4121498399739935</v>
+        <v>0.3805104478604178</v>
       </c>
       <c r="G21" t="n">
-        <v>0.01607788311236881</v>
+        <v>0.01397317757417013</v>
       </c>
       <c r="H21" t="n">
-        <v>0.3069073659722946</v>
+        <v>0.2873350578934022</v>
       </c>
       <c r="I21" t="n">
-        <v>0.002046279153851166</v>
+        <v>0.01137161018286441</v>
       </c>
       <c r="J21" t="n">
-        <v>0.240822059483943</v>
+        <v>0.1988004453461589</v>
       </c>
       <c r="K21" t="n">
-        <v>0.2337086487723459</v>
+        <v>0.2282454299618172</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2337086487723459</v>
+        <v>0.2282454299618172</v>
       </c>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
-        <v>0.2337079080363163</v>
+        <v>0.2282454194978167</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.2337083162283326</v>
+        <v>0.2282454299618172</v>
       </c>
       <c r="R21" t="n">
-        <v>0.2337083162283326</v>
+        <v>0.2282454299618172</v>
       </c>
       <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr"/>
@@ -1872,44 +1872,44 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.005804179144167165</v>
+        <v>0.03591237791649511</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.01713025143721005</v>
+        <v>0.01242534222501369</v>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>-0.03256439045457561</v>
+        <v>-0.003046159129846365</v>
       </c>
       <c r="G22" t="n">
-        <v>0.01543621462186746</v>
+        <v>-0.004196184408110613</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.03583542344941693</v>
+        <v>0.01805804213032168</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.01422955064918202</v>
+        <v>0.007058029146321165</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.04121597302006619</v>
+        <v>-0.006991585011044387</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.03189853903594156</v>
+        <v>0.02248499907539996</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.03189853903594156</v>
+        <v>0.02248499907539996</v>
       </c>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="n">
-        <v>-0.03189910015596401</v>
+        <v>0.02248467037138682</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.03189892533995701</v>
+        <v>0.02248499907539996</v>
       </c>
       <c r="R22" t="n">
-        <v>-0.03189892533995701</v>
+        <v>0.02248499907539996</v>
       </c>
       <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr"/>
@@ -1937,44 +1937,44 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.04447702958708118</v>
+        <v>0.03768182809927311</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.01255258629410345</v>
+        <v>-0.004003539328141572</v>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>0.5324318991212759</v>
+        <v>0.5648460740498429</v>
       </c>
       <c r="G23" t="n">
-        <v>0.01681554191059145</v>
+        <v>0.006732498863373537</v>
       </c>
       <c r="H23" t="n">
-        <v>0.3493670317026812</v>
+        <v>0.3575813793592552</v>
       </c>
       <c r="I23" t="n">
-        <v>0.01575193167007726</v>
+        <v>0.02860057986402319</v>
       </c>
       <c r="J23" t="n">
-        <v>0.4656513342284877</v>
+        <v>0.5073210507675452</v>
       </c>
       <c r="K23" t="n">
-        <v>0.2346401639776065</v>
+        <v>0.2463464564778582</v>
       </c>
       <c r="L23" t="n">
-        <v>0.2346401639776065</v>
+        <v>0.2463464564778582</v>
       </c>
       <c r="M23" t="inlineStr"/>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="n">
-        <v>0.234639350281574</v>
+        <v>0.2463463518378541</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.2346397947615917</v>
+        <v>0.2463464564778582</v>
       </c>
       <c r="R23" t="n">
-        <v>0.2346397947615917</v>
+        <v>0.2463464564778582</v>
       </c>
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
@@ -1998,44 +1998,44 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.04612750322110012</v>
+        <v>0.04515244913409796</v>
       </c>
       <c r="D24" t="n">
-        <v>0.02253726483749059</v>
+        <v>-0.0008729135389165415</v>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>0.6274478860259154</v>
+        <v>0.6143886440635457</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.00812370527106095</v>
+        <v>-0.005579033462587851</v>
       </c>
       <c r="H24" t="n">
-        <v>0.375213551264542</v>
+        <v>0.3878101950324077</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0569299025971961</v>
+        <v>0.03434912921396516</v>
       </c>
       <c r="J24" t="n">
-        <v>0.2763214417699251</v>
+        <v>0.2439418502510377</v>
       </c>
       <c r="K24" t="n">
-        <v>0.2353395222775808</v>
+        <v>0.2691591033743641</v>
       </c>
       <c r="L24" t="n">
-        <v>0.2353395222775808</v>
+        <v>0.2691591033743641</v>
       </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
-        <v>0.2353391611255664</v>
+        <v>0.2691593656463746</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.2353394961655798</v>
+        <v>0.2691591033743641</v>
       </c>
       <c r="R24" t="n">
-        <v>0.2353394961655798</v>
+        <v>0.2691591033743641</v>
       </c>
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
@@ -2063,44 +2063,44 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.05570251202010047</v>
+        <v>0.05572690130107604</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0109187299727492</v>
+        <v>0.01570372123614885</v>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>0.01262806216912249</v>
+        <v>0.02702346175293847</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.03596758070735099</v>
+        <v>-0.02834039813297734</v>
       </c>
       <c r="H25" t="n">
-        <v>0.7339071143802843</v>
+        <v>0.7428746429309856</v>
       </c>
       <c r="I25" t="n">
-        <v>-0.1442909472116379</v>
+        <v>-0.1438246218169849</v>
       </c>
       <c r="J25" t="n">
-        <v>-0.2805631259976858</v>
+        <v>-0.2776638203013536</v>
       </c>
       <c r="K25" t="n">
-        <v>0.8651985131999405</v>
+        <v>0.8631704846068193</v>
       </c>
       <c r="L25" t="n">
-        <v>0.8651985131999405</v>
+        <v>0.8631704846068193</v>
       </c>
       <c r="M25" t="inlineStr"/>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
-        <v>0.8651991897119675</v>
+        <v>0.8631704610868183</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.8651987075039482</v>
+        <v>0.8631704846068193</v>
       </c>
       <c r="R25" t="n">
-        <v>0.8651987075039482</v>
+        <v>0.8631704846068193</v>
       </c>
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
@@ -2124,44 +2124,44 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.020621825048873</v>
+        <v>0.03533937059757482</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.01001658673666347</v>
+        <v>-0.009466703898668154</v>
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>0.01020717717628709</v>
+        <v>-0.01580159016806361</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.009185878879728639</v>
+        <v>0.007869837266799294</v>
       </c>
       <c r="H26" t="n">
-        <v>0.01484679217787168</v>
+        <v>-0.02275145217405809</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.1167475337899013</v>
+        <v>-0.1275863775514551</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.002202676790891927</v>
+        <v>0.006985096322640635</v>
       </c>
       <c r="K26" t="n">
-        <v>0.01434197414167896</v>
+        <v>-0.02152602239704089</v>
       </c>
       <c r="L26" t="n">
-        <v>0.01434197414167896</v>
+        <v>-0.02152602239704089</v>
       </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
-        <v>0.01434230841369234</v>
+        <v>-0.02152614806104592</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.0143421425256857</v>
+        <v>-0.02152602239704089</v>
       </c>
       <c r="R26" t="n">
-        <v>0.0143421425256857</v>
+        <v>-0.02152602239704089</v>
       </c>
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
@@ -2189,44 +2189,44 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.01659769151190766</v>
+        <v>0.001151963374078535</v>
       </c>
       <c r="D27" t="n">
-        <v>0.01890344744413789</v>
+        <v>0.007169562910782515</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>0.005322175124887005</v>
+        <v>0.001759109830364393</v>
       </c>
       <c r="G27" t="n">
-        <v>0.01882737379845932</v>
+        <v>0.009877079648237591</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.004197316679892666</v>
+        <v>0.02526478209859128</v>
       </c>
       <c r="I27" t="n">
-        <v>0.02216655525466221</v>
+        <v>0.001521844956873798</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0055873416061688</v>
+        <v>-0.005189310658899667</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.007608929584357182</v>
+        <v>0.0305934225357369</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.007608929584357182</v>
+        <v>0.0305934225357369</v>
       </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="n">
-        <v>-0.007608734608349383</v>
+        <v>0.03059352141574085</v>
       </c>
       <c r="Q27" t="n">
-        <v>-0.007608856048354241</v>
+        <v>0.0305934225357369</v>
       </c>
       <c r="R27" t="n">
-        <v>-0.007608856048354241</v>
+        <v>0.0305934225357369</v>
       </c>
       <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr"/>
@@ -2254,44 +2254,44 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.003460388586415543</v>
+        <v>0.005386687703467507</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.008152086854083472</v>
+        <v>0.02042471112098844</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="n">
-        <v>0.00825384877815395</v>
+        <v>-0.006659599082383961</v>
       </c>
       <c r="G28" t="n">
-        <v>0.01601739480168638</v>
+        <v>-0.02000724944109788</v>
       </c>
       <c r="H28" t="n">
-        <v>-0.002271765594870623</v>
+        <v>-0.02713225577329023</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.009295592339823692</v>
+        <v>0.03124697328187893</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.01179802838651126</v>
+        <v>0.001456822746649339</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.002362167550486702</v>
+        <v>-0.02846957768278311</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.002362167550486702</v>
+        <v>-0.02846957768278311</v>
       </c>
       <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="n">
-        <v>-0.002361709630468385</v>
+        <v>-0.0284694976187799</v>
       </c>
       <c r="Q28" t="n">
-        <v>-0.002362346014493841</v>
+        <v>-0.02846957768278311</v>
       </c>
       <c r="R28" t="n">
-        <v>-0.002362346014493841</v>
+        <v>-0.02846957768278311</v>
       </c>
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr"/>
@@ -2319,44 +2319,44 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.004290027339601093</v>
+        <v>-0.009201570608062823</v>
       </c>
       <c r="D29" t="n">
-        <v>0.01661224492048979</v>
+        <v>0.01424484632979385</v>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="n">
-        <v>0.00597050375882015</v>
+        <v>-0.007303751812150072</v>
       </c>
       <c r="G29" t="n">
-        <v>-0.01342020554560396</v>
+        <v>-0.00442381736825508</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01008008142720326</v>
+        <v>-0.0010416274976651</v>
       </c>
       <c r="I29" t="n">
-        <v>0.0152566074582643</v>
+        <v>0.01436933673477347</v>
       </c>
       <c r="J29" t="n">
-        <v>0.02266409337194908</v>
+        <v>-0.01534720727496463</v>
       </c>
       <c r="K29" t="n">
-        <v>0.01345922770636911</v>
+        <v>0.000996231975849279</v>
       </c>
       <c r="L29" t="n">
-        <v>0.01345922770636911</v>
+        <v>0.000996231975849279</v>
       </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="n">
-        <v>0.01345858431434337</v>
+        <v>0.0009964375118575002</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.01345925055437002</v>
+        <v>0.000996231975849279</v>
       </c>
       <c r="R29" t="n">
-        <v>0.01345925055437002</v>
+        <v>0.000996231975849279</v>
       </c>
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
@@ -2384,44 +2384,44 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.005655796450231858</v>
+        <v>0.01279103388764135</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.01542497485699899</v>
+        <v>-0.03344480927379236</v>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>-0.005622416096896643</v>
+        <v>0.01490578034023121</v>
       </c>
       <c r="G30" t="n">
-        <v>0.001877693358226282</v>
+        <v>0.007693500003727842</v>
       </c>
       <c r="H30" t="n">
-        <v>0.003365918822636752</v>
+        <v>0.009754593990183757</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.01292798797311952</v>
+        <v>-0.02881285305651412</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.02002661503442991</v>
+        <v>0.004675529858930171</v>
       </c>
       <c r="K30" t="n">
-        <v>0.007794037079761482</v>
+        <v>0.006859257970370319</v>
       </c>
       <c r="L30" t="n">
-        <v>0.007794037079761482</v>
+        <v>0.006859257970370319</v>
       </c>
       <c r="M30" t="inlineStr"/>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="n">
-        <v>0.007794213143768524</v>
+        <v>0.006859317970372718</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.007794142007765679</v>
+        <v>0.006859257970370319</v>
       </c>
       <c r="R30" t="n">
-        <v>0.007794142007765679</v>
+        <v>0.006859257970370319</v>
       </c>
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
@@ -2449,44 +2449,44 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.01340840453633618</v>
+        <v>-0.00543182450527298</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.02025557121022284</v>
+        <v>-0.02334369789374791</v>
       </c>
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="n">
-        <v>-0.004441910673676427</v>
+        <v>0.0007264398050575922</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.01051316810346227</v>
+        <v>-0.0004022310172927133</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.01342320552892822</v>
+        <v>0.005836172873446913</v>
       </c>
       <c r="I31" t="n">
-        <v>-0.0177982724559309</v>
+        <v>-0.02791722812468912</v>
       </c>
       <c r="J31" t="n">
-        <v>-0.0215918403142843</v>
+        <v>0.0044790836067065</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.01003783768151351</v>
+        <v>0.007282886883315474</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.01003783768151351</v>
+        <v>0.007282886883315474</v>
       </c>
       <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="n">
-        <v>-0.01003856430554257</v>
+        <v>0.007283247939329916</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.01003763732950549</v>
+        <v>0.007282886883315474</v>
       </c>
       <c r="R31" t="n">
-        <v>-0.01003763732950549</v>
+        <v>0.007282886883315474</v>
       </c>
       <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr"/>
@@ -2514,44 +2514,44 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.002502678436107137</v>
+        <v>0.01894866632594665</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.01117334454293378</v>
+        <v>-0.002615932040637281</v>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>-0.03400529627221185</v>
+        <v>0.01696761677470467</v>
       </c>
       <c r="G32" t="n">
-        <v>0.0002447481353462698</v>
+        <v>0.005862384550017585</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.02244917331396693</v>
+        <v>0.00846790277071611</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.007829533369181334</v>
+        <v>-0.001938463469538539</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.0162142259849592</v>
+        <v>0.01009029489985851</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.01270947775637911</v>
+        <v>0.004327037837081513</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.01270947775637911</v>
+        <v>0.004327037837081513</v>
       </c>
       <c r="M32" t="inlineStr"/>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="n">
-        <v>-0.01270950415638017</v>
+        <v>0.00432675799707032</v>
       </c>
       <c r="Q32" t="n">
-        <v>-0.01270959737238389</v>
+        <v>0.004327037837081513</v>
       </c>
       <c r="R32" t="n">
-        <v>-0.01270959737238389</v>
+        <v>0.004327037837081513</v>
       </c>
       <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr"/>
@@ -2579,44 +2579,44 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.02960044044801761</v>
+        <v>0.01922648985705959</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.001813062024522481</v>
+        <v>0.01630701386828055</v>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>-0.007309056772362269</v>
+        <v>-0.006994684695787387</v>
       </c>
       <c r="G33" t="n">
-        <v>0.02136498458634498</v>
+        <v>0.01931565920742632</v>
       </c>
       <c r="H33" t="n">
-        <v>0.004344220493768819</v>
+        <v>-0.02462594431303777</v>
       </c>
       <c r="I33" t="n">
-        <v>0.005339030325561212</v>
+        <v>0.01769069801962792</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.005713865389917117</v>
+        <v>0.002758382475637592</v>
       </c>
       <c r="K33" t="n">
-        <v>0.006665496074619842</v>
+        <v>-0.02659425149577006</v>
       </c>
       <c r="L33" t="n">
-        <v>0.006665496074619842</v>
+        <v>-0.02659425149577006</v>
       </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="n">
-        <v>0.00666570401062816</v>
+        <v>-0.02659416384776655</v>
       </c>
       <c r="Q33" t="n">
-        <v>0.006665600618624025</v>
+        <v>-0.02659425149577006</v>
       </c>
       <c r="R33" t="n">
-        <v>0.006665600618624025</v>
+        <v>-0.02659425149577006</v>
       </c>
       <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr"/>
@@ -2644,44 +2644,44 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.01153635598145424</v>
+        <v>0.003427961129118445</v>
       </c>
       <c r="D34" t="n">
-        <v>0.01138237082329483</v>
+        <v>-0.0162324076572963</v>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>-0.008607696056307842</v>
+        <v>-0.01938267475930699</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.02676107481274944</v>
+        <v>-0.02446634743715357</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0004148388645935545</v>
+        <v>-0.03509906521196261</v>
       </c>
       <c r="I34" t="n">
-        <v>0.009421451896858075</v>
+        <v>-0.01124344115373765</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.004691596367313362</v>
+        <v>-0.005558665545882406</v>
       </c>
       <c r="K34" t="n">
-        <v>0.003900743868029754</v>
+        <v>-0.03723331348933253</v>
       </c>
       <c r="L34" t="n">
-        <v>0.003900743868029754</v>
+        <v>-0.03723331348933253</v>
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="n">
-        <v>0.003901428732057149</v>
+        <v>-0.03723340401733615</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.003901068732042749</v>
+        <v>-0.03723331348933253</v>
       </c>
       <c r="R34" t="n">
-        <v>0.003901068732042749</v>
+        <v>-0.03723331348933253</v>
       </c>
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
@@ -2709,44 +2709,44 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.01498248165529926</v>
+        <v>0.0132346701613868</v>
       </c>
       <c r="D35" t="n">
-        <v>0.02218259157530366</v>
+        <v>0.01363320092932804</v>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="n">
-        <v>-0.004281679851267194</v>
+        <v>-0.005867536842701472</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.002839860603496149</v>
+        <v>0.004755152768929411</v>
       </c>
       <c r="H35" t="n">
-        <v>-0.01568360616334424</v>
+        <v>0.00512685601307424</v>
       </c>
       <c r="I35" t="n">
-        <v>0.01903210636128425</v>
+        <v>0.0121781724551269</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.001635301972145893</v>
+        <v>-0.02324897055064394</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.0193938425357537</v>
+        <v>0.008680291259211648</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.0193938425357537</v>
+        <v>0.008680291259211648</v>
       </c>
       <c r="M35" t="inlineStr"/>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="n">
-        <v>-0.01939271338370853</v>
+        <v>0.008680140539205621</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.01939350615174024</v>
+        <v>0.008680291259211648</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.01939350615174024</v>
+        <v>0.008680291259211648</v>
       </c>
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
@@ -2774,44 +2774,44 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.02430466676418667</v>
+        <v>0.004773547198941888</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.002515635364625415</v>
+        <v>-0.009484092667363705</v>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="n">
-        <v>0.01591402978856119</v>
+        <v>-0.005395216919808676</v>
       </c>
       <c r="G36" t="n">
-        <v>0.008878036542668985</v>
+        <v>0.02113547805712719</v>
       </c>
       <c r="H36" t="n">
-        <v>-0.004446259377850374</v>
+        <v>-0.003077592411103696</v>
       </c>
       <c r="I36" t="n">
-        <v>-0.003209677664387106</v>
+        <v>-0.01406126773045071</v>
       </c>
       <c r="J36" t="n">
-        <v>0.004274851653791915</v>
+        <v>0.006108620540102806</v>
       </c>
       <c r="K36" t="n">
-        <v>-0.008410273680410946</v>
+        <v>-0.0006259786810391472</v>
       </c>
       <c r="L36" t="n">
-        <v>-0.008410273680410946</v>
+        <v>-0.0006259786810391472</v>
       </c>
       <c r="M36" t="inlineStr"/>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="n">
-        <v>-0.00841071528042861</v>
+        <v>-0.0006265898170635927</v>
       </c>
       <c r="Q36" t="n">
-        <v>-0.008410539408421574</v>
+        <v>-0.0006259786810391472</v>
       </c>
       <c r="R36" t="n">
-        <v>-0.008410539408421574</v>
+        <v>-0.0006259786810391472</v>
       </c>
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
@@ -2839,44 +2839,44 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.01490312421212497</v>
+        <v>-0.0113114201964568</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.01464582970583318</v>
+        <v>0.0137859299274372</v>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>-0.02571896320475853</v>
+        <v>0.0241137902445516</v>
       </c>
       <c r="G37" t="n">
-        <v>0.007118063202078837</v>
+        <v>-0.004955296150112554</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.02595780430231217</v>
+        <v>0.02540648741625949</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.01236237543849502</v>
+        <v>0.009725492741019708</v>
       </c>
       <c r="J37" t="n">
-        <v>0.003645194575231716</v>
+        <v>0.01614754252476469</v>
       </c>
       <c r="K37" t="n">
-        <v>0.08953490258939609</v>
+        <v>0.02146353676254147</v>
       </c>
       <c r="L37" t="n">
-        <v>0.08953490258939609</v>
+        <v>0.02146353676254147</v>
       </c>
       <c r="M37" t="inlineStr"/>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="n">
-        <v>0.08953467324538691</v>
+        <v>0.02146328063453122</v>
       </c>
       <c r="Q37" t="n">
-        <v>0.08953469830138791</v>
+        <v>0.02146353676254147</v>
       </c>
       <c r="R37" t="n">
-        <v>0.08953469830138791</v>
+        <v>0.02146353676254147</v>
       </c>
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
@@ -2891,6 +2891,71 @@
       <c r="AC37" t="inlineStr"/>
       <c r="AD37" t="inlineStr"/>
       <c r="AE37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>Stream-natural gas</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>GWP [kg*CO2-eq/kg]</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>-0.01375198221407929</v>
+      </c>
+      <c r="D38" t="n">
+        <v>-0.02315309036612361</v>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>-0.005818237384729494</v>
+      </c>
+      <c r="G38" t="n">
+        <v>-0.008804050488192394</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.01355282905411316</v>
+      </c>
+      <c r="I38" t="n">
+        <v>-0.02636794924671797</v>
+      </c>
+      <c r="J38" t="n">
+        <v>-0.008528874722700702</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.09721601102464042</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0.09721601102464042</v>
+      </c>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="n">
+        <v>0.09721561675262465</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0.09721601102464042</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0.09721601102464042</v>
+      </c>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr"/>
+      <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
+      <c r="X38" t="inlineStr"/>
+      <c r="Y38" t="inlineStr"/>
+      <c r="Z38" t="inlineStr"/>
+      <c r="AA38" t="inlineStr"/>
+      <c r="AB38" t="inlineStr"/>
+      <c r="AC38" t="inlineStr"/>
+      <c r="AD38" t="inlineStr"/>
+      <c r="AE38" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>